<commit_message>
add/disambiguate several data format classes
</commit_message>
<xml_diff>
--- a/src/ontology/terms-extraction/cpptraj-10k-occurence_merged.xlsx
+++ b/src/ontology/terms-extraction/cpptraj-10k-occurence_merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\fathoni\github\molsim-ontology\src\ontology\terms-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55248DC7-AB35-47C3-B61A-69E37E2366E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08A33E4-8B84-482D-9D43-C70A0050B302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{41106041-1982-4E74-9156-BB0487A0D691}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="2" xr2:uid="{41106041-1982-4E74-9156-BB0487A0D691}"/>
   </bookViews>
   <sheets>
     <sheet name="deduplicated" sheetId="1" r:id="rId1"/>
@@ -4920,25 +4920,6 @@
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -5056,6 +5037,25 @@
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5070,15 +5070,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C4B6DB4-963D-4C30-A55C-C98D189B16BC}" name="Table1" displayName="Table1" ref="A1:F427" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C4B6DB4-963D-4C30-A55C-C98D189B16BC}" name="Table1" displayName="Table1" ref="A1:F427" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F427" xr:uid="{0C4B6DB4-963D-4C30-A55C-C98D189B16BC}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4773755D-E1AF-448F-B447-27A0AF53A910}" name="SeqNo" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{5400D0B5-7DA4-4FA3-AA49-BBB83134F695}" name="Term" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{594D70C1-00FC-4BDE-8F76-BB819F43268F}" name="Variable" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{7A2D1F6C-9965-4D40-95C3-06D2F350BE72}" name="Description" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{AFD0A349-9A1D-4EC7-B721-75B7F792D66A}" name="Cat1|Cat2|..." dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{1BB5AD3F-1DCC-4382-AAB2-6B0B6D184443}" name="freq" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{4773755D-E1AF-448F-B447-27A0AF53A910}" name="SeqNo" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{5400D0B5-7DA4-4FA3-AA49-BBB83134F695}" name="Term" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{594D70C1-00FC-4BDE-8F76-BB819F43268F}" name="Variable" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{7A2D1F6C-9965-4D40-95C3-06D2F350BE72}" name="Description" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{AFD0A349-9A1D-4EC7-B721-75B7F792D66A}" name="Cat1|Cat2|..." dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{1BB5AD3F-1DCC-4382-AAB2-6B0B6D184443}" name="freq" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16334,8 +16334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBED5332-DFA5-46E1-A3BF-C31FBE96C021}">
   <dimension ref="A1:H427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A415" workbookViewId="0">
-      <selection sqref="A1:F427"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D122" sqref="B122:D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
add missing data format definitions, add terms status sheet
</commit_message>
<xml_diff>
--- a/src/ontology/terms-extraction/cpptraj-10k-occurence_merged.xlsx
+++ b/src/ontology/terms-extraction/cpptraj-10k-occurence_merged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\fathoni\github\molsim-ontology\src\ontology\terms-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DA9EE6-57BB-4488-9F5E-5EC989DB2C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C0DC61-1303-423E-B8D9-664D0892F218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1710" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{41106041-1982-4E74-9156-BB0487A0D691}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5880" uniqueCount="1601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6305" uniqueCount="1600">
   <si>
     <t>Term</t>
   </si>
@@ -4837,9 +4837,6 @@
   </si>
   <si>
     <t>skip? (-=yes)</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -4885,7 +4882,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -4913,20 +4910,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4941,13 +4929,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4980,13 +4965,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -4997,6 +4975,16 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -5022,9 +5010,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5040,25 +5025,6 @@
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -5173,6 +5139,25 @@
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -5357,22 +5342,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42C18C25-2D20-4E1B-9B5E-51A0D85C0CB3}" name="Table13" displayName="Table13" ref="B1:G427" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42C18C25-2D20-4E1B-9B5E-51A0D85C0CB3}" name="Table13" displayName="Table13" ref="B1:G427" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="B1:G427" xr:uid="{42C18C25-2D20-4E1B-9B5E-51A0D85C0CB3}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{DDE9457E-4DB7-438B-9719-987E4EA0E53F}" name="SeqNo" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{C184ED0B-4B92-47F3-8143-13793E62ABC8}" name="Term" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{98037EF8-1E7F-47C4-8EAB-395406751DA4}" name="Variable" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{DF31CB15-8169-4C70-B5D5-24033FEC7253}" name="Description" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{F50EBF01-0CD6-464A-ABA9-250B251F1671}" name="Cat1|Cat2|..." dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{9E567AE2-8551-458F-BFA7-A0D8A467E1B4}" name="freq" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{DDE9457E-4DB7-438B-9719-987E4EA0E53F}" name="SeqNo" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{C184ED0B-4B92-47F3-8143-13793E62ABC8}" name="Term" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{98037EF8-1E7F-47C4-8EAB-395406751DA4}" name="Variable" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{DF31CB15-8169-4C70-B5D5-24033FEC7253}" name="Description" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{F50EBF01-0CD6-464A-ABA9-250B251F1671}" name="Cat1|Cat2|..." dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{9E567AE2-8551-458F-BFA7-A0D8A467E1B4}" name="freq" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{329D34C6-6AFA-4799-96FC-1A9B7A89128F}" name="Table3" displayName="Table3" ref="A1:A427" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{329D34C6-6AFA-4799-96FC-1A9B7A89128F}" name="Table3" displayName="Table3" ref="A1:A427" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2" totalsRowBorderDxfId="1">
   <autoFilter ref="A1:A427" xr:uid="{329D34C6-6AFA-4799-96FC-1A9B7A89128F}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{444B4197-2A6A-4631-9469-9762CA8CBBDD}" name="skip? (-=yes)" dataDxfId="0"/>
@@ -25181,8 +25166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C3501C-AE45-46A7-8757-17633D9B7137}">
   <dimension ref="A1:G427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A430" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25221,7 +25206,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
+      <c r="A2" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -25242,7 +25229,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
@@ -25263,7 +25252,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
@@ -25284,7 +25275,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
+      <c r="A5" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B5" s="3">
         <v>4</v>
       </c>
@@ -25305,7 +25298,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
+      <c r="A6" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B6" s="3">
         <v>5</v>
       </c>
@@ -25326,7 +25321,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
+      <c r="A7" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B7" s="3">
         <v>6</v>
       </c>
@@ -25347,7 +25344,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B8" s="3">
         <v>7</v>
       </c>
@@ -25368,7 +25367,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
+      <c r="A9" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B9" s="3">
         <v>8</v>
       </c>
@@ -25389,7 +25390,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
+      <c r="A10" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B10" s="3">
         <v>9</v>
       </c>
@@ -25410,7 +25413,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
+      <c r="A11" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B11" s="3">
         <v>10</v>
       </c>
@@ -25431,7 +25436,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
+      <c r="A12" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B12" s="3">
         <v>11</v>
       </c>
@@ -25452,7 +25459,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
+      <c r="A13" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B13" s="3">
         <v>12</v>
       </c>
@@ -25473,7 +25482,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
+      <c r="A14" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B14" s="3">
         <v>13</v>
       </c>
@@ -25494,7 +25505,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
+      <c r="A15" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B15" s="3">
         <v>14</v>
       </c>
@@ -25515,7 +25528,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
+      <c r="A16" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B16" s="3">
         <v>15</v>
       </c>
@@ -25536,7 +25551,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
+      <c r="A17" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B17" s="3">
         <v>16</v>
       </c>
@@ -25557,7 +25574,9 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
+      <c r="A18" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B18" s="3">
         <v>17</v>
       </c>
@@ -25578,7 +25597,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="7"/>
+      <c r="A19" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B19" s="3">
         <v>18</v>
       </c>
@@ -25599,7 +25620,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A20" s="7"/>
+      <c r="A20" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B20" s="3">
         <v>19</v>
       </c>
@@ -25620,7 +25643,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="7"/>
+      <c r="A21" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B21" s="3">
         <v>20</v>
       </c>
@@ -25641,7 +25666,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="7"/>
+      <c r="A22" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B22" s="3">
         <v>21</v>
       </c>
@@ -25662,7 +25689,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A23" s="7"/>
+      <c r="A23" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B23" s="3">
         <v>22</v>
       </c>
@@ -25683,7 +25712,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="7"/>
+      <c r="A24" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B24" s="3">
         <v>23</v>
       </c>
@@ -25704,7 +25735,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="7"/>
+      <c r="A25" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B25" s="3">
         <v>24</v>
       </c>
@@ -25725,7 +25758,9 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
+      <c r="A26" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B26" s="3">
         <v>25</v>
       </c>
@@ -25746,7 +25781,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="7"/>
+      <c r="A27" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B27" s="3">
         <v>26</v>
       </c>
@@ -25767,7 +25804,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
+      <c r="A28" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B28" s="3">
         <v>27</v>
       </c>
@@ -25788,7 +25827,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="7"/>
+      <c r="A29" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B29" s="3">
         <v>28</v>
       </c>
@@ -25809,7 +25850,9 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A30" s="7"/>
+      <c r="A30" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B30" s="3">
         <v>29</v>
       </c>
@@ -25830,7 +25873,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="7"/>
+      <c r="A31" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B31" s="3">
         <v>30</v>
       </c>
@@ -25851,7 +25896,9 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="7"/>
+      <c r="A32" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B32" s="3">
         <v>31</v>
       </c>
@@ -25872,7 +25919,9 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="7"/>
+      <c r="A33" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B33" s="3">
         <v>32</v>
       </c>
@@ -25893,7 +25942,9 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A34" s="7"/>
+      <c r="A34" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B34" s="3">
         <v>33</v>
       </c>
@@ -25914,7 +25965,9 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="7"/>
+      <c r="A35" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B35" s="3">
         <v>34</v>
       </c>
@@ -25935,7 +25988,9 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="7"/>
+      <c r="A36" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B36" s="3">
         <v>35</v>
       </c>
@@ -25956,7 +26011,9 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="7"/>
+      <c r="A37" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B37" s="3">
         <v>36</v>
       </c>
@@ -25977,7 +26034,9 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="7"/>
+      <c r="A38" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B38" s="3">
         <v>37</v>
       </c>
@@ -25998,7 +26057,9 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="7"/>
+      <c r="A39" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B39" s="3">
         <v>38</v>
       </c>
@@ -26019,7 +26080,9 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="7"/>
+      <c r="A40" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B40" s="3">
         <v>39</v>
       </c>
@@ -26040,7 +26103,9 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="7"/>
+      <c r="A41" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B41" s="3">
         <v>40</v>
       </c>
@@ -26061,7 +26126,9 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="7"/>
+      <c r="A42" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B42" s="3">
         <v>41</v>
       </c>
@@ -26082,7 +26149,9 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="7"/>
+      <c r="A43" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B43" s="3">
         <v>42</v>
       </c>
@@ -26103,7 +26172,9 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="7"/>
+      <c r="A44" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B44" s="3">
         <v>43</v>
       </c>
@@ -26124,7 +26195,9 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="7"/>
+      <c r="A45" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B45" s="3">
         <v>44</v>
       </c>
@@ -26145,7 +26218,9 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="7"/>
+      <c r="A46" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B46" s="3">
         <v>45</v>
       </c>
@@ -26166,7 +26241,9 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="7"/>
+      <c r="A47" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B47" s="3">
         <v>46</v>
       </c>
@@ -26187,7 +26264,9 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="7"/>
+      <c r="A48" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B48" s="3">
         <v>47</v>
       </c>
@@ -26208,7 +26287,9 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="7"/>
+      <c r="A49" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B49" s="3">
         <v>48</v>
       </c>
@@ -26229,7 +26310,9 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="7"/>
+      <c r="A50" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B50" s="3">
         <v>49</v>
       </c>
@@ -26250,7 +26333,9 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A51" s="7"/>
+      <c r="A51" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B51" s="3">
         <v>50</v>
       </c>
@@ -26271,7 +26356,9 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="7"/>
+      <c r="A52" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B52" s="3">
         <v>51</v>
       </c>
@@ -26292,7 +26379,9 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="7"/>
+      <c r="A53" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B53" s="3">
         <v>52</v>
       </c>
@@ -26313,7 +26402,9 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="7"/>
+      <c r="A54" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B54" s="3">
         <v>53</v>
       </c>
@@ -26334,7 +26425,9 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="7"/>
+      <c r="A55" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B55" s="3">
         <v>54</v>
       </c>
@@ -26355,7 +26448,9 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="7"/>
+      <c r="A56" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B56" s="3">
         <v>55</v>
       </c>
@@ -26376,7 +26471,9 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A57" s="7"/>
+      <c r="A57" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B57" s="3">
         <v>56</v>
       </c>
@@ -26397,7 +26494,9 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="7"/>
+      <c r="A58" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B58" s="3">
         <v>57</v>
       </c>
@@ -26418,7 +26517,9 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="7"/>
+      <c r="A59" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B59" s="3">
         <v>58</v>
       </c>
@@ -26439,7 +26540,9 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="7"/>
+      <c r="A60" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B60" s="3">
         <v>59</v>
       </c>
@@ -26460,7 +26563,9 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="7"/>
+      <c r="A61" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B61" s="3">
         <v>60</v>
       </c>
@@ -26481,7 +26586,9 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="7"/>
+      <c r="A62" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B62" s="3">
         <v>61</v>
       </c>
@@ -26502,7 +26609,9 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="7"/>
+      <c r="A63" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B63" s="3">
         <v>62</v>
       </c>
@@ -26523,7 +26632,9 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A64" s="7"/>
+      <c r="A64" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B64" s="3">
         <v>63</v>
       </c>
@@ -26544,7 +26655,9 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="7"/>
+      <c r="A65" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B65" s="3">
         <v>64</v>
       </c>
@@ -26565,7 +26678,9 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" s="7"/>
+      <c r="A66" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B66" s="3">
         <v>65</v>
       </c>
@@ -26586,7 +26701,9 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="7"/>
+      <c r="A67" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B67" s="3">
         <v>66</v>
       </c>
@@ -26607,7 +26724,9 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" s="7"/>
+      <c r="A68" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B68" s="3">
         <v>67</v>
       </c>
@@ -26628,7 +26747,9 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="7"/>
+      <c r="A69" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B69" s="3">
         <v>68</v>
       </c>
@@ -26649,7 +26770,9 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="7"/>
+      <c r="A70" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B70" s="3">
         <v>69</v>
       </c>
@@ -26670,7 +26793,9 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="7"/>
+      <c r="A71" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B71" s="3">
         <v>70</v>
       </c>
@@ -26691,7 +26816,9 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="7"/>
+      <c r="A72" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B72" s="3">
         <v>71</v>
       </c>
@@ -26712,7 +26839,9 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="7"/>
+      <c r="A73" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B73" s="3">
         <v>72</v>
       </c>
@@ -26733,7 +26862,9 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="7"/>
+      <c r="A74" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B74" s="3">
         <v>73</v>
       </c>
@@ -26754,7 +26885,9 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A75" s="7"/>
+      <c r="A75" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B75" s="3">
         <v>74</v>
       </c>
@@ -26775,7 +26908,9 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76" s="7"/>
+      <c r="A76" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B76" s="3">
         <v>75</v>
       </c>
@@ -26796,7 +26931,9 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A77" s="7"/>
+      <c r="A77" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B77" s="3">
         <v>76</v>
       </c>
@@ -26817,7 +26954,9 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" s="7"/>
+      <c r="A78" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B78" s="3">
         <v>77</v>
       </c>
@@ -26838,7 +26977,9 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" s="7"/>
+      <c r="A79" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B79" s="3">
         <v>78</v>
       </c>
@@ -26859,7 +27000,9 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="7"/>
+      <c r="A80" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B80" s="3">
         <v>79</v>
       </c>
@@ -26880,7 +27023,9 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="7"/>
+      <c r="A81" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B81" s="3">
         <v>80</v>
       </c>
@@ -26901,7 +27046,9 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" s="7"/>
+      <c r="A82" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B82" s="3">
         <v>81</v>
       </c>
@@ -26922,7 +27069,9 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="7"/>
+      <c r="A83" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B83" s="3">
         <v>82</v>
       </c>
@@ -26943,7 +27092,9 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" s="7"/>
+      <c r="A84" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B84" s="3">
         <v>83</v>
       </c>
@@ -26964,7 +27115,9 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" s="7"/>
+      <c r="A85" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B85" s="3">
         <v>84</v>
       </c>
@@ -26985,7 +27138,9 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" s="7"/>
+      <c r="A86" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B86" s="3">
         <v>85</v>
       </c>
@@ -27006,7 +27161,9 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" s="7"/>
+      <c r="A87" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B87" s="3">
         <v>86</v>
       </c>
@@ -27027,7 +27184,9 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="7"/>
+      <c r="A88" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B88" s="3">
         <v>87</v>
       </c>
@@ -27048,7 +27207,9 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" s="7"/>
+      <c r="A89" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B89" s="3">
         <v>88</v>
       </c>
@@ -27069,7 +27230,9 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A90" s="7"/>
+      <c r="A90" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B90" s="3">
         <v>89</v>
       </c>
@@ -27090,7 +27253,9 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91" s="7"/>
+      <c r="A91" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B91" s="3">
         <v>90</v>
       </c>
@@ -27111,7 +27276,9 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92" s="7"/>
+      <c r="A92" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B92" s="3">
         <v>91</v>
       </c>
@@ -27132,7 +27299,9 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" s="7"/>
+      <c r="A93" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B93" s="3">
         <v>92</v>
       </c>
@@ -27153,7 +27322,9 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="7"/>
+      <c r="A94" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B94" s="3">
         <v>93</v>
       </c>
@@ -27174,7 +27345,9 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="7"/>
+      <c r="A95" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B95" s="3">
         <v>94</v>
       </c>
@@ -27195,7 +27368,9 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" s="7"/>
+      <c r="A96" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B96" s="3">
         <v>95</v>
       </c>
@@ -27216,7 +27391,9 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A97" s="7"/>
+      <c r="A97" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B97" s="3">
         <v>96</v>
       </c>
@@ -27237,7 +27414,9 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A98" s="7"/>
+      <c r="A98" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B98" s="3">
         <v>97</v>
       </c>
@@ -27258,7 +27437,9 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A99" s="7"/>
+      <c r="A99" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B99" s="3">
         <v>98</v>
       </c>
@@ -27279,7 +27460,9 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A100" s="7"/>
+      <c r="A100" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B100" s="3">
         <v>99</v>
       </c>
@@ -27300,7 +27483,9 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A101" s="7"/>
+      <c r="A101" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B101" s="3">
         <v>100</v>
       </c>
@@ -27321,7 +27506,9 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A102" s="7"/>
+      <c r="A102" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B102" s="3">
         <v>101</v>
       </c>
@@ -27342,7 +27529,9 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A103" s="7"/>
+      <c r="A103" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B103" s="3">
         <v>102</v>
       </c>
@@ -27363,7 +27552,9 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A104" s="7"/>
+      <c r="A104" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B104" s="3">
         <v>103</v>
       </c>
@@ -27384,7 +27575,9 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A105" s="7"/>
+      <c r="A105" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B105" s="3">
         <v>104</v>
       </c>
@@ -27405,7 +27598,9 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A106" s="7"/>
+      <c r="A106" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B106" s="3">
         <v>105</v>
       </c>
@@ -27426,7 +27621,9 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A107" s="7"/>
+      <c r="A107" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B107" s="3">
         <v>106</v>
       </c>
@@ -27447,7 +27644,9 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A108" s="7"/>
+      <c r="A108" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B108" s="3">
         <v>107</v>
       </c>
@@ -27468,7 +27667,9 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A109" s="7"/>
+      <c r="A109" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B109" s="3">
         <v>108</v>
       </c>
@@ -27489,7 +27690,9 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A110" s="7"/>
+      <c r="A110" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B110" s="3">
         <v>109</v>
       </c>
@@ -27510,7 +27713,9 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A111" s="7"/>
+      <c r="A111" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B111" s="3">
         <v>110</v>
       </c>
@@ -27531,7 +27736,9 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A112" s="7"/>
+      <c r="A112" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B112" s="3">
         <v>111</v>
       </c>
@@ -27552,7 +27759,9 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A113" s="7"/>
+      <c r="A113" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B113" s="3">
         <v>112</v>
       </c>
@@ -27573,7 +27782,9 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A114" s="7"/>
+      <c r="A114" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B114" s="3">
         <v>113</v>
       </c>
@@ -27594,7 +27805,9 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A115" s="7"/>
+      <c r="A115" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B115" s="3">
         <v>114</v>
       </c>
@@ -27615,7 +27828,9 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A116" s="7"/>
+      <c r="A116" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B116" s="3">
         <v>115</v>
       </c>
@@ -27636,7 +27851,9 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A117" s="7"/>
+      <c r="A117" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B117" s="3">
         <v>116</v>
       </c>
@@ -27657,7 +27874,9 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A118" s="7"/>
+      <c r="A118" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B118" s="3">
         <v>117</v>
       </c>
@@ -27678,7 +27897,9 @@
       </c>
     </row>
     <row r="119" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A119" s="7"/>
+      <c r="A119" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B119" s="3">
         <v>118</v>
       </c>
@@ -27699,7 +27920,9 @@
       </c>
     </row>
     <row r="120" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A120" s="7"/>
+      <c r="A120" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B120" s="3">
         <v>119</v>
       </c>
@@ -27720,7 +27943,9 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" s="7"/>
+      <c r="A121" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B121" s="3">
         <v>120</v>
       </c>
@@ -27741,7 +27966,9 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A122" s="7"/>
+      <c r="A122" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B122" s="3">
         <v>121</v>
       </c>
@@ -27762,7 +27989,9 @@
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A123" s="7"/>
+      <c r="A123" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B123" s="3">
         <v>122</v>
       </c>
@@ -27783,7 +28012,9 @@
       </c>
     </row>
     <row r="124" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A124" s="7"/>
+      <c r="A124" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B124" s="3">
         <v>123</v>
       </c>
@@ -27804,7 +28035,9 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A125" s="7"/>
+      <c r="A125" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B125" s="3">
         <v>124</v>
       </c>
@@ -27825,7 +28058,9 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A126" s="7"/>
+      <c r="A126" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B126" s="3">
         <v>125</v>
       </c>
@@ -27846,7 +28081,9 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A127" s="7"/>
+      <c r="A127" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B127" s="3">
         <v>126</v>
       </c>
@@ -27867,7 +28104,9 @@
       </c>
     </row>
     <row r="128" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A128" s="7"/>
+      <c r="A128" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B128" s="3">
         <v>127</v>
       </c>
@@ -27888,7 +28127,9 @@
       </c>
     </row>
     <row r="129" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A129" s="7"/>
+      <c r="A129" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B129" s="3">
         <v>128</v>
       </c>
@@ -27909,7 +28150,9 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A130" s="7"/>
+      <c r="A130" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B130" s="3">
         <v>129</v>
       </c>
@@ -27930,7 +28173,9 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A131" s="7"/>
+      <c r="A131" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B131" s="3">
         <v>130</v>
       </c>
@@ -27951,7 +28196,9 @@
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A132" s="7"/>
+      <c r="A132" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B132" s="3">
         <v>131</v>
       </c>
@@ -27972,7 +28219,9 @@
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A133" s="7"/>
+      <c r="A133" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B133" s="3">
         <v>132</v>
       </c>
@@ -27993,7 +28242,9 @@
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A134" s="7"/>
+      <c r="A134" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B134" s="3">
         <v>133</v>
       </c>
@@ -28014,7 +28265,9 @@
       </c>
     </row>
     <row r="135" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A135" s="7"/>
+      <c r="A135" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B135" s="3">
         <v>134</v>
       </c>
@@ -28035,7 +28288,9 @@
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A136" s="7"/>
+      <c r="A136" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B136" s="3">
         <v>135</v>
       </c>
@@ -28056,7 +28311,9 @@
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A137" s="7"/>
+      <c r="A137" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B137" s="3">
         <v>136</v>
       </c>
@@ -28077,7 +28334,9 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A138" s="7"/>
+      <c r="A138" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B138" s="3">
         <v>137</v>
       </c>
@@ -28098,7 +28357,9 @@
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A139" s="7"/>
+      <c r="A139" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B139" s="3">
         <v>138</v>
       </c>
@@ -28119,7 +28380,9 @@
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A140" s="7"/>
+      <c r="A140" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B140" s="3">
         <v>139</v>
       </c>
@@ -28140,7 +28403,9 @@
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A141" s="7"/>
+      <c r="A141" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B141" s="3">
         <v>140</v>
       </c>
@@ -28161,7 +28426,9 @@
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A142" s="7"/>
+      <c r="A142" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B142" s="3">
         <v>141</v>
       </c>
@@ -28182,7 +28449,9 @@
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A143" s="7"/>
+      <c r="A143" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B143" s="3">
         <v>142</v>
       </c>
@@ -28203,7 +28472,9 @@
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A144" s="7"/>
+      <c r="A144" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B144" s="3">
         <v>143</v>
       </c>
@@ -28224,7 +28495,9 @@
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A145" s="7"/>
+      <c r="A145" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B145" s="3">
         <v>144</v>
       </c>
@@ -28245,7 +28518,9 @@
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A146" s="7"/>
+      <c r="A146" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B146" s="3">
         <v>145</v>
       </c>
@@ -28266,7 +28541,9 @@
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A147" s="7"/>
+      <c r="A147" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B147" s="3">
         <v>146</v>
       </c>
@@ -28287,7 +28564,9 @@
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A148" s="7"/>
+      <c r="A148" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B148" s="3">
         <v>147</v>
       </c>
@@ -28308,7 +28587,9 @@
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A149" s="7"/>
+      <c r="A149" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B149" s="3">
         <v>148</v>
       </c>
@@ -28329,7 +28610,9 @@
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A150" s="7"/>
+      <c r="A150" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B150" s="3">
         <v>149</v>
       </c>
@@ -28350,7 +28633,9 @@
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A151" s="7"/>
+      <c r="A151" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B151" s="3">
         <v>150</v>
       </c>
@@ -28371,7 +28656,9 @@
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A152" s="7"/>
+      <c r="A152" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B152" s="3">
         <v>151</v>
       </c>
@@ -28392,7 +28679,9 @@
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A153" s="7"/>
+      <c r="A153" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B153" s="3">
         <v>152</v>
       </c>
@@ -28413,7 +28702,9 @@
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A154" s="7"/>
+      <c r="A154" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B154" s="3">
         <v>153</v>
       </c>
@@ -28434,7 +28725,9 @@
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A155" s="7"/>
+      <c r="A155" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B155" s="3">
         <v>154</v>
       </c>
@@ -28455,7 +28748,9 @@
       </c>
     </row>
     <row r="156" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A156" s="7"/>
+      <c r="A156" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B156" s="3">
         <v>155</v>
       </c>
@@ -28476,7 +28771,9 @@
       </c>
     </row>
     <row r="157" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A157" s="7"/>
+      <c r="A157" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B157" s="3">
         <v>156</v>
       </c>
@@ -28497,7 +28794,9 @@
       </c>
     </row>
     <row r="158" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A158" s="7"/>
+      <c r="A158" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B158" s="3">
         <v>157</v>
       </c>
@@ -28518,7 +28817,9 @@
       </c>
     </row>
     <row r="159" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A159" s="7"/>
+      <c r="A159" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B159" s="3">
         <v>158</v>
       </c>
@@ -28539,7 +28840,9 @@
       </c>
     </row>
     <row r="160" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A160" s="7"/>
+      <c r="A160" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B160" s="3">
         <v>159</v>
       </c>
@@ -28560,7 +28863,9 @@
       </c>
     </row>
     <row r="161" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A161" s="7"/>
+      <c r="A161" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B161" s="3">
         <v>160</v>
       </c>
@@ -28581,7 +28886,9 @@
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A162" s="7"/>
+      <c r="A162" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B162" s="3">
         <v>161</v>
       </c>
@@ -28602,7 +28909,9 @@
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A163" s="7"/>
+      <c r="A163" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B163" s="3">
         <v>162</v>
       </c>
@@ -28623,7 +28932,9 @@
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A164" s="7"/>
+      <c r="A164" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B164" s="3">
         <v>163</v>
       </c>
@@ -28644,7 +28955,9 @@
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A165" s="7"/>
+      <c r="A165" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B165" s="3">
         <v>164</v>
       </c>
@@ -28665,7 +28978,9 @@
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A166" s="7"/>
+      <c r="A166" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B166" s="3">
         <v>165</v>
       </c>
@@ -28686,7 +29001,9 @@
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A167" s="7"/>
+      <c r="A167" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B167" s="3">
         <v>166</v>
       </c>
@@ -28707,7 +29024,9 @@
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A168" s="7"/>
+      <c r="A168" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B168" s="3">
         <v>167</v>
       </c>
@@ -28728,7 +29047,9 @@
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A169" s="7"/>
+      <c r="A169" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B169" s="3">
         <v>168</v>
       </c>
@@ -28749,7 +29070,9 @@
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A170" s="7"/>
+      <c r="A170" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B170" s="3">
         <v>169</v>
       </c>
@@ -28770,7 +29093,9 @@
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A171" s="7"/>
+      <c r="A171" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B171" s="3">
         <v>170</v>
       </c>
@@ -28791,7 +29116,9 @@
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A172" s="7"/>
+      <c r="A172" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B172" s="3">
         <v>171</v>
       </c>
@@ -28812,7 +29139,9 @@
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A173" s="7"/>
+      <c r="A173" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B173" s="3">
         <v>172</v>
       </c>
@@ -28833,7 +29162,9 @@
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A174" s="7"/>
+      <c r="A174" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B174" s="3">
         <v>173</v>
       </c>
@@ -28854,7 +29185,9 @@
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A175" s="7"/>
+      <c r="A175" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B175" s="3">
         <v>174</v>
       </c>
@@ -28875,7 +29208,9 @@
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A176" s="7"/>
+      <c r="A176" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B176" s="3">
         <v>175</v>
       </c>
@@ -28896,7 +29231,9 @@
       </c>
     </row>
     <row r="177" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A177" s="7"/>
+      <c r="A177" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B177" s="3">
         <v>176</v>
       </c>
@@ -28917,7 +29254,9 @@
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A178" s="7"/>
+      <c r="A178" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B178" s="3">
         <v>177</v>
       </c>
@@ -28938,7 +29277,9 @@
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A179" s="7"/>
+      <c r="A179" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B179" s="3">
         <v>178</v>
       </c>
@@ -28959,7 +29300,9 @@
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A180" s="7"/>
+      <c r="A180" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B180" s="3">
         <v>179</v>
       </c>
@@ -28980,7 +29323,9 @@
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A181" s="7"/>
+      <c r="A181" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B181" s="3">
         <v>180</v>
       </c>
@@ -29001,7 +29346,9 @@
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A182" s="7"/>
+      <c r="A182" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B182" s="3">
         <v>181</v>
       </c>
@@ -29022,7 +29369,9 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A183" s="7"/>
+      <c r="A183" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B183" s="3">
         <v>182</v>
       </c>
@@ -29043,7 +29392,9 @@
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A184" s="7"/>
+      <c r="A184" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B184" s="3">
         <v>183</v>
       </c>
@@ -29064,7 +29415,9 @@
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A185" s="7"/>
+      <c r="A185" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B185" s="3">
         <v>184</v>
       </c>
@@ -29085,7 +29438,9 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A186" s="7"/>
+      <c r="A186" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B186" s="3">
         <v>185</v>
       </c>
@@ -29106,7 +29461,9 @@
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A187" s="7"/>
+      <c r="A187" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B187" s="3">
         <v>186</v>
       </c>
@@ -29127,7 +29484,9 @@
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A188" s="7"/>
+      <c r="A188" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B188" s="3">
         <v>187</v>
       </c>
@@ -29148,7 +29507,9 @@
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A189" s="7"/>
+      <c r="A189" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B189" s="3">
         <v>188</v>
       </c>
@@ -29169,7 +29530,9 @@
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A190" s="7"/>
+      <c r="A190" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B190" s="3">
         <v>189</v>
       </c>
@@ -29190,7 +29553,9 @@
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A191" s="7"/>
+      <c r="A191" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B191" s="3">
         <v>190</v>
       </c>
@@ -29211,7 +29576,9 @@
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A192" s="7"/>
+      <c r="A192" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B192" s="3">
         <v>191</v>
       </c>
@@ -29232,7 +29599,9 @@
       </c>
     </row>
     <row r="193" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A193" s="7"/>
+      <c r="A193" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B193" s="3">
         <v>192</v>
       </c>
@@ -29253,7 +29622,9 @@
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A194" s="7"/>
+      <c r="A194" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B194" s="3">
         <v>193</v>
       </c>
@@ -29274,7 +29645,9 @@
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A195" s="7"/>
+      <c r="A195" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B195" s="3">
         <v>194</v>
       </c>
@@ -29295,7 +29668,9 @@
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A196" s="7"/>
+      <c r="A196" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B196" s="3">
         <v>195</v>
       </c>
@@ -29316,7 +29691,9 @@
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A197" s="7"/>
+      <c r="A197" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B197" s="3">
         <v>196</v>
       </c>
@@ -29337,7 +29714,9 @@
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A198" s="7"/>
+      <c r="A198" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B198" s="3">
         <v>197</v>
       </c>
@@ -29358,7 +29737,9 @@
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A199" s="7"/>
+      <c r="A199" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B199" s="3">
         <v>198</v>
       </c>
@@ -29379,7 +29760,9 @@
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A200" s="7"/>
+      <c r="A200" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B200" s="3">
         <v>199</v>
       </c>
@@ -29400,7 +29783,9 @@
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A201" s="7"/>
+      <c r="A201" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B201" s="3">
         <v>200</v>
       </c>
@@ -29421,7 +29806,9 @@
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A202" s="7"/>
+      <c r="A202" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B202" s="3">
         <v>201</v>
       </c>
@@ -29442,7 +29829,9 @@
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A203" s="7"/>
+      <c r="A203" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B203" s="3">
         <v>202</v>
       </c>
@@ -29463,7 +29852,9 @@
       </c>
     </row>
     <row r="204" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A204" s="7"/>
+      <c r="A204" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B204" s="3">
         <v>203</v>
       </c>
@@ -29484,7 +29875,9 @@
       </c>
     </row>
     <row r="205" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A205" s="7"/>
+      <c r="A205" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B205" s="3">
         <v>204</v>
       </c>
@@ -29505,7 +29898,9 @@
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A206" s="7"/>
+      <c r="A206" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B206" s="3">
         <v>205</v>
       </c>
@@ -29526,7 +29921,9 @@
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A207" s="7"/>
+      <c r="A207" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B207" s="3">
         <v>206</v>
       </c>
@@ -29547,7 +29944,9 @@
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A208" s="7"/>
+      <c r="A208" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B208" s="3">
         <v>207</v>
       </c>
@@ -29568,7 +29967,9 @@
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A209" s="7"/>
+      <c r="A209" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B209" s="3">
         <v>208</v>
       </c>
@@ -29589,7 +29990,9 @@
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A210" s="7"/>
+      <c r="A210" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B210" s="3">
         <v>209</v>
       </c>
@@ -29610,7 +30013,9 @@
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A211" s="7"/>
+      <c r="A211" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B211" s="3">
         <v>210</v>
       </c>
@@ -29631,7 +30036,9 @@
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A212" s="7"/>
+      <c r="A212" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B212" s="3">
         <v>211</v>
       </c>
@@ -29652,7 +30059,9 @@
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A213" s="7"/>
+      <c r="A213" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B213" s="3">
         <v>212</v>
       </c>
@@ -29673,7 +30082,9 @@
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A214" s="7"/>
+      <c r="A214" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B214" s="3">
         <v>213</v>
       </c>
@@ -29694,7 +30105,9 @@
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A215" s="7"/>
+      <c r="A215" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B215" s="3">
         <v>214</v>
       </c>
@@ -29715,7 +30128,9 @@
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A216" s="7"/>
+      <c r="A216" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B216" s="3">
         <v>215</v>
       </c>
@@ -29736,7 +30151,9 @@
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A217" s="7"/>
+      <c r="A217" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B217" s="3">
         <v>216</v>
       </c>
@@ -29757,7 +30174,9 @@
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A218" s="7"/>
+      <c r="A218" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B218" s="3">
         <v>217</v>
       </c>
@@ -29778,7 +30197,9 @@
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A219" s="7"/>
+      <c r="A219" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B219" s="3">
         <v>218</v>
       </c>
@@ -29799,7 +30220,9 @@
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A220" s="7"/>
+      <c r="A220" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B220" s="3">
         <v>219</v>
       </c>
@@ -29820,7 +30243,9 @@
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A221" s="7"/>
+      <c r="A221" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B221" s="3">
         <v>220</v>
       </c>
@@ -29841,7 +30266,9 @@
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A222" s="7"/>
+      <c r="A222" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B222" s="3">
         <v>221</v>
       </c>
@@ -29862,7 +30289,9 @@
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A223" s="7"/>
+      <c r="A223" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B223" s="3">
         <v>222</v>
       </c>
@@ -29883,7 +30312,9 @@
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A224" s="7"/>
+      <c r="A224" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B224" s="3">
         <v>223</v>
       </c>
@@ -29904,7 +30335,9 @@
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A225" s="7"/>
+      <c r="A225" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B225" s="3">
         <v>224</v>
       </c>
@@ -29925,7 +30358,9 @@
       </c>
     </row>
     <row r="226" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A226" s="7"/>
+      <c r="A226" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B226" s="3">
         <v>225</v>
       </c>
@@ -29946,7 +30381,9 @@
       </c>
     </row>
     <row r="227" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A227" s="7"/>
+      <c r="A227" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B227" s="3">
         <v>226</v>
       </c>
@@ -29967,7 +30404,9 @@
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A228" s="7"/>
+      <c r="A228" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B228" s="3">
         <v>227</v>
       </c>
@@ -29988,7 +30427,9 @@
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A229" s="7"/>
+      <c r="A229" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B229" s="3">
         <v>228</v>
       </c>
@@ -30009,7 +30450,9 @@
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A230" s="7"/>
+      <c r="A230" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B230" s="3">
         <v>229</v>
       </c>
@@ -30030,7 +30473,9 @@
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A231" s="7"/>
+      <c r="A231" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B231" s="3">
         <v>230</v>
       </c>
@@ -30051,7 +30496,9 @@
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A232" s="7"/>
+      <c r="A232" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B232" s="3">
         <v>231</v>
       </c>
@@ -30072,7 +30519,9 @@
       </c>
     </row>
     <row r="233" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A233" s="7"/>
+      <c r="A233" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B233" s="3">
         <v>232</v>
       </c>
@@ -30093,7 +30542,9 @@
       </c>
     </row>
     <row r="234" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A234" s="7"/>
+      <c r="A234" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B234" s="3">
         <v>233</v>
       </c>
@@ -30114,7 +30565,9 @@
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A235" s="7"/>
+      <c r="A235" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B235" s="3">
         <v>234</v>
       </c>
@@ -30135,7 +30588,9 @@
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A236" s="7"/>
+      <c r="A236" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B236" s="3">
         <v>235</v>
       </c>
@@ -30156,7 +30611,9 @@
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A237" s="7"/>
+      <c r="A237" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B237" s="3">
         <v>236</v>
       </c>
@@ -30177,7 +30634,9 @@
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A238" s="7"/>
+      <c r="A238" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B238" s="3">
         <v>237</v>
       </c>
@@ -30198,7 +30657,9 @@
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A239" s="7"/>
+      <c r="A239" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B239" s="3">
         <v>238</v>
       </c>
@@ -30219,7 +30680,9 @@
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A240" s="7"/>
+      <c r="A240" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B240" s="3">
         <v>239</v>
       </c>
@@ -30240,7 +30703,9 @@
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A241" s="7"/>
+      <c r="A241" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B241" s="3">
         <v>240</v>
       </c>
@@ -30261,7 +30726,9 @@
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A242" s="7"/>
+      <c r="A242" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B242" s="3">
         <v>241</v>
       </c>
@@ -30282,7 +30749,9 @@
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A243" s="7"/>
+      <c r="A243" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B243" s="3">
         <v>242</v>
       </c>
@@ -30303,7 +30772,9 @@
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A244" s="7"/>
+      <c r="A244" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B244" s="3">
         <v>243</v>
       </c>
@@ -30324,7 +30795,9 @@
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A245" s="7"/>
+      <c r="A245" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B245" s="3">
         <v>244</v>
       </c>
@@ -30345,7 +30818,9 @@
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A246" s="7"/>
+      <c r="A246" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B246" s="3">
         <v>245</v>
       </c>
@@ -30366,7 +30841,9 @@
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A247" s="7"/>
+      <c r="A247" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B247" s="3">
         <v>246</v>
       </c>
@@ -30387,7 +30864,9 @@
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A248" s="7"/>
+      <c r="A248" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B248" s="3">
         <v>247</v>
       </c>
@@ -30408,7 +30887,9 @@
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A249" s="7"/>
+      <c r="A249" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B249" s="3">
         <v>248</v>
       </c>
@@ -30429,7 +30910,9 @@
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A250" s="7"/>
+      <c r="A250" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B250" s="3">
         <v>249</v>
       </c>
@@ -30450,7 +30933,9 @@
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A251" s="7"/>
+      <c r="A251" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B251" s="3">
         <v>250</v>
       </c>
@@ -30471,7 +30956,9 @@
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A252" s="7"/>
+      <c r="A252" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B252" s="3">
         <v>251</v>
       </c>
@@ -30492,7 +30979,9 @@
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A253" s="7"/>
+      <c r="A253" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B253" s="3">
         <v>252</v>
       </c>
@@ -30513,7 +31002,9 @@
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A254" s="7"/>
+      <c r="A254" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B254" s="3">
         <v>253</v>
       </c>
@@ -30534,7 +31025,9 @@
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A255" s="7"/>
+      <c r="A255" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B255" s="3">
         <v>254</v>
       </c>
@@ -30555,7 +31048,9 @@
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A256" s="7"/>
+      <c r="A256" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B256" s="3">
         <v>255</v>
       </c>
@@ -30576,7 +31071,9 @@
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A257" s="7"/>
+      <c r="A257" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B257" s="3">
         <v>256</v>
       </c>
@@ -30597,7 +31094,9 @@
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A258" s="7"/>
+      <c r="A258" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B258" s="3">
         <v>257</v>
       </c>
@@ -30618,7 +31117,9 @@
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A259" s="7"/>
+      <c r="A259" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B259" s="3">
         <v>258</v>
       </c>
@@ -30639,7 +31140,9 @@
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A260" s="7"/>
+      <c r="A260" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B260" s="3">
         <v>259</v>
       </c>
@@ -30660,7 +31163,9 @@
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A261" s="7"/>
+      <c r="A261" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B261" s="3">
         <v>260</v>
       </c>
@@ -30681,7 +31186,9 @@
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A262" s="7"/>
+      <c r="A262" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B262" s="3">
         <v>261</v>
       </c>
@@ -30702,7 +31209,9 @@
       </c>
     </row>
     <row r="263" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A263" s="7"/>
+      <c r="A263" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B263" s="3">
         <v>262</v>
       </c>
@@ -30723,7 +31232,9 @@
       </c>
     </row>
     <row r="264" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A264" s="7"/>
+      <c r="A264" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B264" s="3">
         <v>263</v>
       </c>
@@ -30744,7 +31255,9 @@
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A265" s="7"/>
+      <c r="A265" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B265" s="3">
         <v>264</v>
       </c>
@@ -30765,7 +31278,9 @@
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A266" s="7"/>
+      <c r="A266" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B266" s="3">
         <v>265</v>
       </c>
@@ -30786,7 +31301,9 @@
       </c>
     </row>
     <row r="267" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A267" s="7"/>
+      <c r="A267" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B267" s="3">
         <v>266</v>
       </c>
@@ -30807,7 +31324,9 @@
       </c>
     </row>
     <row r="268" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A268" s="7"/>
+      <c r="A268" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B268" s="3">
         <v>267</v>
       </c>
@@ -30828,7 +31347,9 @@
       </c>
     </row>
     <row r="269" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A269" s="7"/>
+      <c r="A269" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B269" s="3">
         <v>268</v>
       </c>
@@ -30849,7 +31370,9 @@
       </c>
     </row>
     <row r="270" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A270" s="7"/>
+      <c r="A270" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B270" s="3">
         <v>269</v>
       </c>
@@ -30870,7 +31393,9 @@
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A271" s="7"/>
+      <c r="A271" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B271" s="3">
         <v>270</v>
       </c>
@@ -30891,7 +31416,9 @@
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A272" s="7"/>
+      <c r="A272" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B272" s="3">
         <v>271</v>
       </c>
@@ -30912,7 +31439,9 @@
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A273" s="7"/>
+      <c r="A273" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B273" s="3">
         <v>272</v>
       </c>
@@ -30933,7 +31462,9 @@
       </c>
     </row>
     <row r="274" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A274" s="7"/>
+      <c r="A274" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B274" s="3">
         <v>273</v>
       </c>
@@ -30954,7 +31485,9 @@
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A275" s="7"/>
+      <c r="A275" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B275" s="3">
         <v>274</v>
       </c>
@@ -30975,7 +31508,9 @@
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A276" s="7"/>
+      <c r="A276" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B276" s="3">
         <v>275</v>
       </c>
@@ -30996,7 +31531,9 @@
       </c>
     </row>
     <row r="277" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A277" s="7"/>
+      <c r="A277" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B277" s="3">
         <v>276</v>
       </c>
@@ -31017,7 +31554,9 @@
       </c>
     </row>
     <row r="278" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A278" s="7"/>
+      <c r="A278" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B278" s="3">
         <v>277</v>
       </c>
@@ -31038,7 +31577,9 @@
       </c>
     </row>
     <row r="279" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A279" s="7"/>
+      <c r="A279" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B279" s="3">
         <v>278</v>
       </c>
@@ -31059,7 +31600,9 @@
       </c>
     </row>
     <row r="280" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A280" s="7"/>
+      <c r="A280" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B280" s="3">
         <v>279</v>
       </c>
@@ -31080,7 +31623,9 @@
       </c>
     </row>
     <row r="281" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A281" s="7"/>
+      <c r="A281" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B281" s="3">
         <v>280</v>
       </c>
@@ -31101,7 +31646,9 @@
       </c>
     </row>
     <row r="282" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A282" s="7"/>
+      <c r="A282" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B282" s="3">
         <v>281</v>
       </c>
@@ -31122,7 +31669,9 @@
       </c>
     </row>
     <row r="283" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A283" s="7"/>
+      <c r="A283" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B283" s="3">
         <v>282</v>
       </c>
@@ -31143,7 +31692,9 @@
       </c>
     </row>
     <row r="284" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A284" s="7"/>
+      <c r="A284" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B284" s="3">
         <v>283</v>
       </c>
@@ -31164,7 +31715,9 @@
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A285" s="7"/>
+      <c r="A285" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B285" s="3">
         <v>284</v>
       </c>
@@ -31185,7 +31738,9 @@
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A286" s="7"/>
+      <c r="A286" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B286" s="3">
         <v>285</v>
       </c>
@@ -31206,7 +31761,9 @@
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A287" s="7"/>
+      <c r="A287" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B287" s="3">
         <v>286</v>
       </c>
@@ -31227,7 +31784,9 @@
       </c>
     </row>
     <row r="288" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A288" s="7"/>
+      <c r="A288" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B288" s="3">
         <v>287</v>
       </c>
@@ -31248,7 +31807,9 @@
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A289" s="7"/>
+      <c r="A289" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B289" s="3">
         <v>288</v>
       </c>
@@ -31269,7 +31830,9 @@
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A290" s="7"/>
+      <c r="A290" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B290" s="3">
         <v>289</v>
       </c>
@@ -31290,7 +31853,9 @@
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A291" s="7"/>
+      <c r="A291" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B291" s="3">
         <v>290</v>
       </c>
@@ -31311,7 +31876,9 @@
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A292" s="7"/>
+      <c r="A292" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B292" s="3">
         <v>291</v>
       </c>
@@ -31332,7 +31899,9 @@
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A293" s="7"/>
+      <c r="A293" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B293" s="3">
         <v>292</v>
       </c>
@@ -31353,7 +31922,9 @@
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A294" s="7"/>
+      <c r="A294" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B294" s="3">
         <v>293</v>
       </c>
@@ -31374,7 +31945,9 @@
       </c>
     </row>
     <row r="295" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A295" s="7"/>
+      <c r="A295" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B295" s="3">
         <v>294</v>
       </c>
@@ -31395,7 +31968,9 @@
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A296" s="7"/>
+      <c r="A296" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B296" s="3">
         <v>295</v>
       </c>
@@ -31416,7 +31991,9 @@
       </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A297" s="7"/>
+      <c r="A297" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B297" s="3">
         <v>296</v>
       </c>
@@ -31437,7 +32014,9 @@
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A298" s="7"/>
+      <c r="A298" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B298" s="3">
         <v>297</v>
       </c>
@@ -31458,7 +32037,9 @@
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A299" s="7"/>
+      <c r="A299" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B299" s="3">
         <v>298</v>
       </c>
@@ -31479,7 +32060,9 @@
       </c>
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A300" s="7"/>
+      <c r="A300" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B300" s="3">
         <v>299</v>
       </c>
@@ -31500,7 +32083,9 @@
       </c>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A301" s="7"/>
+      <c r="A301" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B301" s="3">
         <v>300</v>
       </c>
@@ -31521,7 +32106,9 @@
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A302" s="7"/>
+      <c r="A302" s="7" t="s">
+        <v>599</v>
+      </c>
       <c r="B302" s="3">
         <v>301</v>
       </c>
@@ -31542,8 +32129,8 @@
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A303" s="7" t="s">
-        <v>1600</v>
+      <c r="A303" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="B303" s="3">
         <v>302</v>
@@ -31565,7 +32152,9 @@
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A304" s="7"/>
+      <c r="A304" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B304" s="3">
         <v>303</v>
       </c>
@@ -31586,7 +32175,9 @@
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A305" s="7"/>
+      <c r="A305" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B305" s="3">
         <v>304</v>
       </c>
@@ -31607,7 +32198,9 @@
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A306" s="7"/>
+      <c r="A306" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B306" s="3">
         <v>305</v>
       </c>
@@ -31628,7 +32221,9 @@
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A307" s="7"/>
+      <c r="A307" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B307" s="3">
         <v>306</v>
       </c>
@@ -31649,7 +32244,9 @@
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A308" s="7"/>
+      <c r="A308" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B308" s="3">
         <v>307</v>
       </c>
@@ -31670,7 +32267,9 @@
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A309" s="7"/>
+      <c r="A309" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B309" s="3">
         <v>308</v>
       </c>
@@ -31691,7 +32290,9 @@
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A310" s="7"/>
+      <c r="A310" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B310" s="3">
         <v>309</v>
       </c>
@@ -31712,7 +32313,9 @@
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A311" s="7"/>
+      <c r="A311" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B311" s="3">
         <v>310</v>
       </c>
@@ -31733,7 +32336,9 @@
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A312" s="7"/>
+      <c r="A312" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B312" s="3">
         <v>311</v>
       </c>
@@ -31754,7 +32359,9 @@
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A313" s="7"/>
+      <c r="A313" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B313" s="3">
         <v>312</v>
       </c>
@@ -31775,7 +32382,9 @@
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A314" s="7"/>
+      <c r="A314" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B314" s="3">
         <v>313</v>
       </c>
@@ -31796,7 +32405,9 @@
       </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A315" s="7"/>
+      <c r="A315" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B315" s="3">
         <v>314</v>
       </c>
@@ -31817,7 +32428,9 @@
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A316" s="7"/>
+      <c r="A316" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B316" s="3">
         <v>315</v>
       </c>
@@ -31838,7 +32451,9 @@
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A317" s="7"/>
+      <c r="A317" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B317" s="3">
         <v>316</v>
       </c>
@@ -31859,7 +32474,9 @@
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A318" s="7"/>
+      <c r="A318" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B318" s="3">
         <v>317</v>
       </c>
@@ -31880,7 +32497,9 @@
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A319" s="7"/>
+      <c r="A319" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B319" s="3">
         <v>318</v>
       </c>
@@ -31901,7 +32520,9 @@
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A320" s="7"/>
+      <c r="A320" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B320" s="3">
         <v>319</v>
       </c>
@@ -31922,7 +32543,9 @@
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A321" s="7"/>
+      <c r="A321" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B321" s="3">
         <v>320</v>
       </c>
@@ -31943,7 +32566,9 @@
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A322" s="7"/>
+      <c r="A322" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B322" s="3">
         <v>321</v>
       </c>
@@ -31964,7 +32589,9 @@
       </c>
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A323" s="7"/>
+      <c r="A323" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B323" s="3">
         <v>322</v>
       </c>
@@ -31985,7 +32612,9 @@
       </c>
     </row>
     <row r="324" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A324" s="7"/>
+      <c r="A324" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B324" s="3">
         <v>323</v>
       </c>
@@ -32006,7 +32635,9 @@
       </c>
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A325" s="7"/>
+      <c r="A325" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B325" s="3">
         <v>324</v>
       </c>
@@ -32027,7 +32658,9 @@
       </c>
     </row>
     <row r="326" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A326" s="7"/>
+      <c r="A326" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B326" s="3">
         <v>325</v>
       </c>
@@ -32048,7 +32681,9 @@
       </c>
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A327" s="7"/>
+      <c r="A327" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B327" s="3">
         <v>326</v>
       </c>
@@ -32069,7 +32704,9 @@
       </c>
     </row>
     <row r="328" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A328" s="7"/>
+      <c r="A328" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B328" s="3">
         <v>327</v>
       </c>
@@ -32090,7 +32727,9 @@
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A329" s="7"/>
+      <c r="A329" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B329" s="3">
         <v>328</v>
       </c>
@@ -32111,7 +32750,9 @@
       </c>
     </row>
     <row r="330" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A330" s="7"/>
+      <c r="A330" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B330" s="3">
         <v>329</v>
       </c>
@@ -32132,7 +32773,9 @@
       </c>
     </row>
     <row r="331" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A331" s="7"/>
+      <c r="A331" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B331" s="3">
         <v>330</v>
       </c>
@@ -32153,7 +32796,9 @@
       </c>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A332" s="7"/>
+      <c r="A332" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B332" s="3">
         <v>331</v>
       </c>
@@ -32174,7 +32819,9 @@
       </c>
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A333" s="7"/>
+      <c r="A333" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B333" s="3">
         <v>332</v>
       </c>
@@ -32195,7 +32842,9 @@
       </c>
     </row>
     <row r="334" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A334" s="7"/>
+      <c r="A334" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B334" s="3">
         <v>333</v>
       </c>
@@ -32216,7 +32865,9 @@
       </c>
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A335" s="7"/>
+      <c r="A335" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B335" s="3">
         <v>334</v>
       </c>
@@ -32237,7 +32888,9 @@
       </c>
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A336" s="7"/>
+      <c r="A336" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B336" s="3">
         <v>335</v>
       </c>
@@ -32258,7 +32911,9 @@
       </c>
     </row>
     <row r="337" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A337" s="7"/>
+      <c r="A337" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B337" s="3">
         <v>336</v>
       </c>
@@ -32279,7 +32934,9 @@
       </c>
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A338" s="7"/>
+      <c r="A338" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B338" s="3">
         <v>337</v>
       </c>
@@ -32300,7 +32957,9 @@
       </c>
     </row>
     <row r="339" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A339" s="7"/>
+      <c r="A339" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B339" s="3">
         <v>338</v>
       </c>
@@ -32321,7 +32980,9 @@
       </c>
     </row>
     <row r="340" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A340" s="7"/>
+      <c r="A340" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B340" s="3">
         <v>339</v>
       </c>
@@ -32342,7 +33003,9 @@
       </c>
     </row>
     <row r="341" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A341" s="7"/>
+      <c r="A341" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B341" s="3">
         <v>340</v>
       </c>
@@ -32363,7 +33026,9 @@
       </c>
     </row>
     <row r="342" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A342" s="7"/>
+      <c r="A342" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B342" s="3">
         <v>341</v>
       </c>
@@ -32384,7 +33049,9 @@
       </c>
     </row>
     <row r="343" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A343" s="7"/>
+      <c r="A343" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B343" s="3">
         <v>342</v>
       </c>
@@ -32405,7 +33072,9 @@
       </c>
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A344" s="7"/>
+      <c r="A344" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B344" s="3">
         <v>343</v>
       </c>
@@ -32426,7 +33095,9 @@
       </c>
     </row>
     <row r="345" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A345" s="7"/>
+      <c r="A345" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B345" s="3">
         <v>344</v>
       </c>
@@ -32447,7 +33118,9 @@
       </c>
     </row>
     <row r="346" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A346" s="7"/>
+      <c r="A346" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B346" s="3">
         <v>345</v>
       </c>
@@ -32468,7 +33141,9 @@
       </c>
     </row>
     <row r="347" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A347" s="7"/>
+      <c r="A347" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B347" s="3">
         <v>346</v>
       </c>
@@ -32489,7 +33164,9 @@
       </c>
     </row>
     <row r="348" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A348" s="7"/>
+      <c r="A348" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B348" s="3">
         <v>347</v>
       </c>
@@ -32510,7 +33187,9 @@
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A349" s="7"/>
+      <c r="A349" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B349" s="3">
         <v>348</v>
       </c>
@@ -32531,7 +33210,9 @@
       </c>
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A350" s="7"/>
+      <c r="A350" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B350" s="3">
         <v>349</v>
       </c>
@@ -32552,7 +33233,9 @@
       </c>
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A351" s="7"/>
+      <c r="A351" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B351" s="3">
         <v>350</v>
       </c>
@@ -32573,7 +33256,9 @@
       </c>
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A352" s="7"/>
+      <c r="A352" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B352" s="3">
         <v>351</v>
       </c>
@@ -32594,7 +33279,9 @@
       </c>
     </row>
     <row r="353" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A353" s="7"/>
+      <c r="A353" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B353" s="3">
         <v>352</v>
       </c>
@@ -32615,7 +33302,9 @@
       </c>
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A354" s="7"/>
+      <c r="A354" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B354" s="3">
         <v>353</v>
       </c>
@@ -32636,7 +33325,9 @@
       </c>
     </row>
     <row r="355" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A355" s="7"/>
+      <c r="A355" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B355" s="3">
         <v>354</v>
       </c>
@@ -32657,7 +33348,9 @@
       </c>
     </row>
     <row r="356" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A356" s="7"/>
+      <c r="A356" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B356" s="3">
         <v>355</v>
       </c>
@@ -32678,7 +33371,9 @@
       </c>
     </row>
     <row r="357" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A357" s="7"/>
+      <c r="A357" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B357" s="3">
         <v>356</v>
       </c>
@@ -32699,7 +33394,9 @@
       </c>
     </row>
     <row r="358" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A358" s="7"/>
+      <c r="A358" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B358" s="3">
         <v>357</v>
       </c>
@@ -32720,7 +33417,9 @@
       </c>
     </row>
     <row r="359" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A359" s="7"/>
+      <c r="A359" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B359" s="3">
         <v>358</v>
       </c>
@@ -32741,7 +33440,9 @@
       </c>
     </row>
     <row r="360" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A360" s="7"/>
+      <c r="A360" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B360" s="3">
         <v>359</v>
       </c>
@@ -32762,7 +33463,9 @@
       </c>
     </row>
     <row r="361" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A361" s="7"/>
+      <c r="A361" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B361" s="3">
         <v>360</v>
       </c>
@@ -32783,7 +33486,9 @@
       </c>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A362" s="7"/>
+      <c r="A362" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B362" s="3">
         <v>361</v>
       </c>
@@ -32804,7 +33509,9 @@
       </c>
     </row>
     <row r="363" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A363" s="7"/>
+      <c r="A363" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B363" s="3">
         <v>362</v>
       </c>
@@ -32825,7 +33532,9 @@
       </c>
     </row>
     <row r="364" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A364" s="7"/>
+      <c r="A364" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B364" s="3">
         <v>363</v>
       </c>
@@ -32846,7 +33555,9 @@
       </c>
     </row>
     <row r="365" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A365" s="7"/>
+      <c r="A365" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B365" s="3">
         <v>364</v>
       </c>
@@ -32867,7 +33578,9 @@
       </c>
     </row>
     <row r="366" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A366" s="7"/>
+      <c r="A366" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B366" s="3">
         <v>365</v>
       </c>
@@ -32888,7 +33601,9 @@
       </c>
     </row>
     <row r="367" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A367" s="7"/>
+      <c r="A367" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B367" s="3">
         <v>366</v>
       </c>
@@ -32909,7 +33624,9 @@
       </c>
     </row>
     <row r="368" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A368" s="7"/>
+      <c r="A368" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B368" s="3">
         <v>367</v>
       </c>
@@ -32930,7 +33647,9 @@
       </c>
     </row>
     <row r="369" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A369" s="7"/>
+      <c r="A369" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B369" s="3">
         <v>368</v>
       </c>
@@ -32951,7 +33670,9 @@
       </c>
     </row>
     <row r="370" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A370" s="7"/>
+      <c r="A370" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B370" s="3">
         <v>369</v>
       </c>
@@ -32972,7 +33693,9 @@
       </c>
     </row>
     <row r="371" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A371" s="7"/>
+      <c r="A371" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B371" s="3">
         <v>370</v>
       </c>
@@ -32993,7 +33716,9 @@
       </c>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A372" s="7"/>
+      <c r="A372" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B372" s="3">
         <v>371</v>
       </c>
@@ -33014,7 +33739,9 @@
       </c>
     </row>
     <row r="373" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A373" s="7"/>
+      <c r="A373" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B373" s="3">
         <v>372</v>
       </c>
@@ -33035,7 +33762,9 @@
       </c>
     </row>
     <row r="374" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A374" s="7"/>
+      <c r="A374" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B374" s="3">
         <v>373</v>
       </c>
@@ -33056,7 +33785,9 @@
       </c>
     </row>
     <row r="375" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A375" s="7"/>
+      <c r="A375" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B375" s="3">
         <v>374</v>
       </c>
@@ -33077,7 +33808,9 @@
       </c>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A376" s="7"/>
+      <c r="A376" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B376" s="3">
         <v>375</v>
       </c>
@@ -33098,7 +33831,9 @@
       </c>
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A377" s="7"/>
+      <c r="A377" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B377" s="3">
         <v>376</v>
       </c>
@@ -33119,7 +33854,9 @@
       </c>
     </row>
     <row r="378" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A378" s="7"/>
+      <c r="A378" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B378" s="3">
         <v>377</v>
       </c>
@@ -33140,7 +33877,9 @@
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A379" s="7"/>
+      <c r="A379" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B379" s="3">
         <v>378</v>
       </c>
@@ -33161,7 +33900,9 @@
       </c>
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A380" s="7"/>
+      <c r="A380" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B380" s="3">
         <v>379</v>
       </c>
@@ -33182,7 +33923,9 @@
       </c>
     </row>
     <row r="381" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A381" s="7"/>
+      <c r="A381" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B381" s="3">
         <v>380</v>
       </c>
@@ -33203,7 +33946,9 @@
       </c>
     </row>
     <row r="382" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A382" s="7"/>
+      <c r="A382" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B382" s="3">
         <v>381</v>
       </c>
@@ -33224,7 +33969,9 @@
       </c>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A383" s="7"/>
+      <c r="A383" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B383" s="3">
         <v>382</v>
       </c>
@@ -33245,7 +33992,9 @@
       </c>
     </row>
     <row r="384" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A384" s="7"/>
+      <c r="A384" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B384" s="3">
         <v>383</v>
       </c>
@@ -33266,7 +34015,9 @@
       </c>
     </row>
     <row r="385" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A385" s="7"/>
+      <c r="A385" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B385" s="3">
         <v>384</v>
       </c>
@@ -33287,7 +34038,9 @@
       </c>
     </row>
     <row r="386" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A386" s="7"/>
+      <c r="A386" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B386" s="3">
         <v>385</v>
       </c>
@@ -33308,7 +34061,9 @@
       </c>
     </row>
     <row r="387" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A387" s="7"/>
+      <c r="A387" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B387" s="3">
         <v>386</v>
       </c>
@@ -33329,7 +34084,9 @@
       </c>
     </row>
     <row r="388" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A388" s="7"/>
+      <c r="A388" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B388" s="3">
         <v>387</v>
       </c>
@@ -33350,7 +34107,9 @@
       </c>
     </row>
     <row r="389" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A389" s="7"/>
+      <c r="A389" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B389" s="3">
         <v>388</v>
       </c>
@@ -33371,7 +34130,9 @@
       </c>
     </row>
     <row r="390" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A390" s="7"/>
+      <c r="A390" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B390" s="3">
         <v>389</v>
       </c>
@@ -33392,7 +34153,9 @@
       </c>
     </row>
     <row r="391" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A391" s="7"/>
+      <c r="A391" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B391" s="3">
         <v>390</v>
       </c>
@@ -33413,7 +34176,9 @@
       </c>
     </row>
     <row r="392" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A392" s="7"/>
+      <c r="A392" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B392" s="3">
         <v>391</v>
       </c>
@@ -33434,7 +34199,9 @@
       </c>
     </row>
     <row r="393" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A393" s="7"/>
+      <c r="A393" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B393" s="3">
         <v>392</v>
       </c>
@@ -33455,7 +34222,9 @@
       </c>
     </row>
     <row r="394" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A394" s="7"/>
+      <c r="A394" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B394" s="3">
         <v>393</v>
       </c>
@@ -33476,7 +34245,9 @@
       </c>
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A395" s="7"/>
+      <c r="A395" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B395" s="3">
         <v>394</v>
       </c>
@@ -33497,7 +34268,9 @@
       </c>
     </row>
     <row r="396" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A396" s="7"/>
+      <c r="A396" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B396" s="3">
         <v>395</v>
       </c>
@@ -33518,7 +34291,9 @@
       </c>
     </row>
     <row r="397" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A397" s="7"/>
+      <c r="A397" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B397" s="3">
         <v>396</v>
       </c>
@@ -33539,7 +34314,9 @@
       </c>
     </row>
     <row r="398" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A398" s="7"/>
+      <c r="A398" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B398" s="3">
         <v>397</v>
       </c>
@@ -33560,7 +34337,9 @@
       </c>
     </row>
     <row r="399" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A399" s="7"/>
+      <c r="A399" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B399" s="3">
         <v>398</v>
       </c>
@@ -33581,7 +34360,9 @@
       </c>
     </row>
     <row r="400" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A400" s="7"/>
+      <c r="A400" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B400" s="3">
         <v>399</v>
       </c>
@@ -33602,7 +34383,9 @@
       </c>
     </row>
     <row r="401" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A401" s="7"/>
+      <c r="A401" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B401" s="3">
         <v>400</v>
       </c>
@@ -33623,7 +34406,9 @@
       </c>
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A402" s="7"/>
+      <c r="A402" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B402" s="3">
         <v>401</v>
       </c>
@@ -33644,7 +34429,9 @@
       </c>
     </row>
     <row r="403" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A403" s="7"/>
+      <c r="A403" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B403" s="3">
         <v>402</v>
       </c>
@@ -33665,7 +34452,9 @@
       </c>
     </row>
     <row r="404" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A404" s="7"/>
+      <c r="A404" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B404" s="3">
         <v>403</v>
       </c>
@@ -33686,7 +34475,9 @@
       </c>
     </row>
     <row r="405" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A405" s="7"/>
+      <c r="A405" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B405" s="3">
         <v>404</v>
       </c>
@@ -33707,7 +34498,9 @@
       </c>
     </row>
     <row r="406" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A406" s="7"/>
+      <c r="A406" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B406" s="3">
         <v>405</v>
       </c>
@@ -33728,7 +34521,9 @@
       </c>
     </row>
     <row r="407" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A407" s="7"/>
+      <c r="A407" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B407" s="3">
         <v>406</v>
       </c>
@@ -33749,7 +34544,9 @@
       </c>
     </row>
     <row r="408" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A408" s="7"/>
+      <c r="A408" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B408" s="3">
         <v>407</v>
       </c>
@@ -33770,7 +34567,9 @@
       </c>
     </row>
     <row r="409" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A409" s="7"/>
+      <c r="A409" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B409" s="3">
         <v>408</v>
       </c>
@@ -33791,7 +34590,9 @@
       </c>
     </row>
     <row r="410" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A410" s="7"/>
+      <c r="A410" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B410" s="3">
         <v>409</v>
       </c>
@@ -33812,7 +34613,9 @@
       </c>
     </row>
     <row r="411" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A411" s="7"/>
+      <c r="A411" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B411" s="3">
         <v>410</v>
       </c>
@@ -33833,7 +34636,9 @@
       </c>
     </row>
     <row r="412" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A412" s="7"/>
+      <c r="A412" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B412" s="3">
         <v>411</v>
       </c>
@@ -33854,7 +34659,9 @@
       </c>
     </row>
     <row r="413" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A413" s="7"/>
+      <c r="A413" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B413" s="3">
         <v>412</v>
       </c>
@@ -33875,7 +34682,9 @@
       </c>
     </row>
     <row r="414" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A414" s="7"/>
+      <c r="A414" s="6" t="s">
+        <v>599</v>
+      </c>
       <c r="B414" s="3">
         <v>413</v>
       </c>
@@ -33896,8 +34705,12 @@
       </c>
     </row>
     <row r="415" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A415" s="7"/>
-      <c r="B415" s="3"/>
+      <c r="A415" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B415" s="3">
+        <v>414</v>
+      </c>
       <c r="C415" s="3" t="s">
         <v>1539</v>
       </c>
@@ -33915,8 +34728,12 @@
       </c>
     </row>
     <row r="416" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A416" s="7"/>
-      <c r="B416" s="3"/>
+      <c r="A416" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B416" s="3">
+        <v>415</v>
+      </c>
       <c r="C416" s="3" t="s">
         <v>1544</v>
       </c>
@@ -33934,8 +34751,12 @@
       </c>
     </row>
     <row r="417" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A417" s="7"/>
-      <c r="B417" s="3"/>
+      <c r="A417" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B417" s="3">
+        <v>416</v>
+      </c>
       <c r="C417" s="3" t="s">
         <v>1549</v>
       </c>
@@ -33953,8 +34774,12 @@
       </c>
     </row>
     <row r="418" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A418" s="7"/>
-      <c r="B418" s="3"/>
+      <c r="A418" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B418" s="3">
+        <v>417</v>
+      </c>
       <c r="C418" s="3" t="s">
         <v>1554</v>
       </c>
@@ -33972,8 +34797,12 @@
       </c>
     </row>
     <row r="419" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A419" s="7"/>
-      <c r="B419" s="3"/>
+      <c r="A419" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B419" s="3">
+        <v>418</v>
+      </c>
       <c r="C419" s="3" t="s">
         <v>1559</v>
       </c>
@@ -33991,8 +34820,12 @@
       </c>
     </row>
     <row r="420" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A420" s="7"/>
-      <c r="B420" s="3"/>
+      <c r="A420" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B420" s="3">
+        <v>419</v>
+      </c>
       <c r="C420" s="3" t="s">
         <v>1563</v>
       </c>
@@ -34010,8 +34843,12 @@
       </c>
     </row>
     <row r="421" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A421" s="7"/>
-      <c r="B421" s="3"/>
+      <c r="A421" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B421" s="3">
+        <v>420</v>
+      </c>
       <c r="C421" s="3" t="s">
         <v>1568</v>
       </c>
@@ -34029,8 +34866,12 @@
       </c>
     </row>
     <row r="422" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A422" s="7"/>
-      <c r="B422" s="3"/>
+      <c r="A422" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B422" s="3">
+        <v>421</v>
+      </c>
       <c r="C422" s="3" t="s">
         <v>1573</v>
       </c>
@@ -34048,8 +34889,12 @@
       </c>
     </row>
     <row r="423" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A423" s="7"/>
-      <c r="B423" s="3"/>
+      <c r="A423" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B423" s="3">
+        <v>422</v>
+      </c>
       <c r="C423" s="3" t="s">
         <v>1578</v>
       </c>
@@ -34067,8 +34912,12 @@
       </c>
     </row>
     <row r="424" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A424" s="7"/>
-      <c r="B424" s="3"/>
+      <c r="A424" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B424" s="3">
+        <v>423</v>
+      </c>
       <c r="C424" s="3" t="s">
         <v>1583</v>
       </c>
@@ -34086,8 +34935,12 @@
       </c>
     </row>
     <row r="425" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A425" s="7"/>
-      <c r="B425" s="3"/>
+      <c r="A425" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B425" s="3">
+        <v>424</v>
+      </c>
       <c r="C425" s="3" t="s">
         <v>1587</v>
       </c>
@@ -34105,8 +34958,12 @@
       </c>
     </row>
     <row r="426" spans="1:7" ht="25" x14ac:dyDescent="0.35">
-      <c r="A426" s="7"/>
-      <c r="B426" s="3"/>
+      <c r="A426" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B426" s="3">
+        <v>425</v>
+      </c>
       <c r="C426" s="3" t="s">
         <v>1592</v>
       </c>
@@ -34124,8 +34981,12 @@
       </c>
     </row>
     <row r="427" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A427" s="8"/>
-      <c r="B427" s="3"/>
+      <c r="A427" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B427" s="3">
+        <v>426</v>
+      </c>
       <c r="C427" s="3" t="s">
         <v>1596</v>
       </c>

</xml_diff>

<commit_message>
add missing definitions for software classes
</commit_message>
<xml_diff>
--- a/src/ontology/terms-extraction/cpptraj-10k-occurence_merged.xlsx
+++ b/src/ontology/terms-extraction/cpptraj-10k-occurence_merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\fathoni\github\molsim-ontology\src\ontology\terms-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C0DC61-1303-423E-B8D9-664D0892F218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A522B0B2-41EC-4F5B-86BB-04DC22D30E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{41106041-1982-4E74-9156-BB0487A0D691}"/>
+    <workbookView xWindow="1500" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{41106041-1982-4E74-9156-BB0487A0D691}"/>
   </bookViews>
   <sheets>
     <sheet name="deduplicated" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -17390,7 +17393,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="25" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -17490,7 +17493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="25" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -18150,7 +18153,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="25" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -19130,7 +19133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="25" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -24490,7 +24493,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="394" spans="1:6" ht="25" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A394" s="3">
         <v>393</v>
       </c>
@@ -24967,7 +24970,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="418" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A418" s="3"/>
       <c r="B418" s="3" t="s">
         <v>1554</v>
@@ -25166,8 +25169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C3501C-AE45-46A7-8757-17633D9B7137}">
   <dimension ref="A1:G427"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A397" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E402" sqref="E402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>